<commit_message>
check_derived_variables.R: updated function compares PARAM and PARAMN columns in specs file with output dataset. recode_ATPT.R: extracts the greater value for ranges. recode_VISIT.R: extracts varied data formats for 'week' and 'day' data with flanking strings.
</commit_message>
<xml_diff>
--- a/tests/data-raw/specs.xlsx
+++ b/tests/data-raw/specs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Human Predictions\1. Resource\Github\standardization\tests\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Human Predictions\1. Resource\8. Github-package development\1. contd. standardization\updates\index_Nov28\standardization\tests\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACFFFC6-0E52-4766-A6DE-9D44F907FB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5D9764-77C7-426C-88E9-E1C34D006F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A04CF2D8-168F-4E34-8EF1-E1A6AB0D100D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A04CF2D8-168F-4E34-8EF1-E1A6AB0D100D}"/>
   </bookViews>
   <sheets>
     <sheet name="Specification-Source Data" sheetId="3" r:id="rId1"/>
+    <sheet name="Recode PARAM" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Specification-Source Data'!$A$1:$F$8</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="81">
   <si>
     <t>Column Name</t>
   </si>
@@ -266,6 +267,21 @@
   </si>
   <si>
     <t>Character, ISO8601 Date-Time</t>
+  </si>
+  <si>
+    <t>PARAM</t>
+  </si>
+  <si>
+    <t>PARAMN</t>
+  </si>
+  <si>
+    <t>EVID</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>Hemoglobin</t>
   </si>
 </sst>
 </file>
@@ -309,8 +325,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,29 +645,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA02D774-3D36-47C9-84D6-20FAA2DE4E2D}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="66.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="39.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
       <c r="D1" t="s">
@@ -662,348 +680,348 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1014,7 +1032,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37308ACA-8A5A-4FF9-ACCE-AA7B5189C112}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ccdc7be-04a4-4bd9-95aa-8d746301efb5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d1c5290-332c-4a39-a7c3-8cc2cd68c520" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1023,7 +1109,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF357BFCA7E8224A8A7DD58544E45F26" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="189e8c2298f7ea2a3e4c7ded2d08a893">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d1c5290-332c-4a39-a7c3-8cc2cd68c520" xmlns:ns3="4ccdc7be-04a4-4bd9-95aa-8d746301efb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="96f4c70b748875eb4ebf57c7af7f9aab" ns2:_="" ns3:_="">
     <xsd:import namespace="0d1c5290-332c-4a39-a7c3-8cc2cd68c520"/>
@@ -1266,18 +1352,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ccdc7be-04a4-4bd9-95aa-8d746301efb5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d1c5290-332c-4a39-a7c3-8cc2cd68c520" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF703263-BF67-426F-AC40-742351CA63C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ccdc7be-04a4-4bd9-95aa-8d746301efb5"/>
+    <ds:schemaRef ds:uri="0d1c5290-332c-4a39-a7c3-8cc2cd68c520"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F248C24-97FC-48A4-844F-A699A9BA9ADD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1285,7 +1371,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6BD364-06FD-4280-BCE3-B25539FBCF91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1302,15 +1388,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF703263-BF67-426F-AC40-742351CA63C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ccdc7be-04a4-4bd9-95aa-8d746301efb5"/>
-    <ds:schemaRef ds:uri="0d1c5290-332c-4a39-a7c3-8cc2cd68c520"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated recode_VISIT.R and documentation
</commit_message>
<xml_diff>
--- a/tests/data-raw/specs.xlsx
+++ b/tests/data-raw/specs.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Human Predictions\1. Resource\8. Github-package development\1. contd. standardization\updates\index_Nov28\standardization\tests\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Human Predictions\1. Resource\8. Github-package development\1. contd. standardization\standardization\tests\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5D9764-77C7-426C-88E9-E1C34D006F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8283E44-D079-4D3E-B995-CBF2E71DF06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A04CF2D8-168F-4E34-8EF1-E1A6AB0D100D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A04CF2D8-168F-4E34-8EF1-E1A6AB0D100D}"/>
   </bookViews>
   <sheets>
     <sheet name="Specification-Source Data" sheetId="3" r:id="rId1"/>
     <sheet name="Recode PARAM" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Specification-Source Data'!$A$1:$F$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Specification-Source Data'!$A$1:$F$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -173,9 +173,6 @@
     <t>ATPT</t>
   </si>
   <si>
-    <t>PCTPT,FATPT,VSTPT,EGTPT</t>
-  </si>
-  <si>
     <t>Planned Time Point Name</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>Hemoglobin</t>
+  </si>
+  <si>
+    <t>PCTPT,EXTPT,FATPT,VSTPT,EGTPT</t>
   </si>
 </sst>
 </file>
@@ -347,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -387,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -493,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -635,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -645,9 +645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA02D774-3D36-47C9-84D6-20FAA2DE4E2D}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,13 +870,13 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
       </c>
       <c r="E12" t="s">
         <v>42</v>
@@ -887,59 +887,59 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" t="s">
         <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
       </c>
       <c r="E14" t="s">
         <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
         <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>58</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
@@ -947,19 +947,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
@@ -967,19 +967,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="D17" t="s">
-        <v>66</v>
-      </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
@@ -987,19 +987,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" t="s">
         <v>69</v>
       </c>
-      <c r="D18" t="s">
-        <v>70</v>
-      </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -1007,26 +1007,26 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
-        <v>74</v>
-      </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F8" xr:uid="{BA02D774-3D36-47C9-84D6-20FAA2DE4E2D}"/>
+  <autoFilter ref="A1:F19" xr:uid="{BA02D774-3D36-47C9-84D6-20FAA2DE4E2D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1036,8 +1036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37308ACA-8A5A-4FF9-ACCE-AA7B5189C112}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,18 +1047,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>77</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1090,26 +1090,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ccdc7be-04a4-4bd9-95aa-8d746301efb5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d1c5290-332c-4a39-a7c3-8cc2cd68c520" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF357BFCA7E8224A8A7DD58544E45F26" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="189e8c2298f7ea2a3e4c7ded2d08a893">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d1c5290-332c-4a39-a7c3-8cc2cd68c520" xmlns:ns3="4ccdc7be-04a4-4bd9-95aa-8d746301efb5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="96f4c70b748875eb4ebf57c7af7f9aab" ns2:_="" ns3:_="">
     <xsd:import namespace="0d1c5290-332c-4a39-a7c3-8cc2cd68c520"/>
@@ -1352,26 +1332,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF703263-BF67-426F-AC40-742351CA63C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ccdc7be-04a4-4bd9-95aa-8d746301efb5"/>
-    <ds:schemaRef ds:uri="0d1c5290-332c-4a39-a7c3-8cc2cd68c520"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F248C24-97FC-48A4-844F-A699A9BA9ADD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4ccdc7be-04a4-4bd9-95aa-8d746301efb5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d1c5290-332c-4a39-a7c3-8cc2cd68c520" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A6BD364-06FD-4280-BCE3-B25539FBCF91}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1388,4 +1369,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F248C24-97FC-48A4-844F-A699A9BA9ADD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF703263-BF67-426F-AC40-742351CA63C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ccdc7be-04a4-4bd9-95aa-8d746301efb5"/>
+    <ds:schemaRef ds:uri="0d1c5290-332c-4a39-a7c3-8cc2cd68c520"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>